<commit_message>
ajustes de precios especiales
</commit_message>
<xml_diff>
--- a/Recursos/Listado_Categorias_Y_Otros.xlsx
+++ b/Recursos/Listado_Categorias_Y_Otros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\medirex-app\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EA18A2-5ECD-49A9-8A59-23764B6728EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CCB11A-1C54-4986-A49B-0D5DC82E77A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A05AB6B-72A9-4425-96EA-FB82AB4FF5BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A05AB6B-72A9-4425-96EA-FB82AB4FF5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -730,18 +730,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907A75D9-58C4-46DC-978A-36AF87F0C678}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.7109375" customWidth="1"/>
-    <col min="5" max="5" width="57.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.6640625" customWidth="1"/>
+    <col min="5" max="5" width="57.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,7 +760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -775,7 +777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -790,7 +792,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -805,7 +807,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -820,7 +822,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -835,7 +837,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -850,7 +852,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -865,7 +867,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -880,7 +882,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -895,7 +897,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -910,7 +912,7 @@
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -925,7 +927,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
@@ -940,7 +942,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
@@ -955,7 +957,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
@@ -970,7 +972,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
@@ -985,7 +987,7 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
@@ -1000,7 +1002,7 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
@@ -1015,7 +1017,7 @@
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
@@ -1030,7 +1032,7 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
@@ -1045,7 +1047,7 @@
       </c>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>45</v>
       </c>
@@ -1060,7 +1062,7 @@
       </c>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>47</v>
       </c>
@@ -1075,7 +1077,7 @@
       </c>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
@@ -1090,7 +1092,7 @@
       </c>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>53</v>
       </c>
@@ -1105,7 +1107,7 @@
       </c>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>55</v>
       </c>
@@ -1120,7 +1122,7 @@
       </c>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>58</v>
       </c>
@@ -1135,7 +1137,7 @@
       </c>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>61</v>
       </c>
@@ -1150,7 +1152,7 @@
       </c>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>63</v>
       </c>
@@ -1165,7 +1167,7 @@
       </c>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>65</v>
       </c>
@@ -1180,7 +1182,7 @@
       </c>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>65</v>
       </c>
@@ -1195,7 +1197,7 @@
       </c>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>65</v>
       </c>
@@ -1210,7 +1212,7 @@
       </c>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>72</v>
       </c>
@@ -1225,7 +1227,7 @@
       </c>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>72</v>
       </c>
@@ -1240,7 +1242,7 @@
       </c>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>77</v>
       </c>
@@ -1255,7 +1257,7 @@
       </c>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>77</v>
       </c>
@@ -1270,7 +1272,7 @@
       </c>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>77</v>
       </c>
@@ -1285,7 +1287,7 @@
       </c>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>77</v>
       </c>
@@ -1300,7 +1302,7 @@
       </c>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>86</v>
       </c>
@@ -1315,7 +1317,7 @@
       </c>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>89</v>
       </c>
@@ -1330,7 +1332,7 @@
       </c>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>91</v>
       </c>
@@ -1345,7 +1347,7 @@
       </c>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>93</v>
       </c>

</xml_diff>